<commit_message>
analysis up to 20230425
</commit_message>
<xml_diff>
--- a/Wound_Closure/Output/summary.table.combined.xlsx
+++ b/Wound_Closure/Output/summary.table.combined.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninahmunk/Desktop/Projects/Acropora_Regeneration-main/Wound_Closure/Output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D98774-8C11-7B4E-91AC-FAB0448038B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5BFEC20-958F-3A49-85EE-529919CACE6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="3400" windowWidth="32880" windowHeight="17180" xr2:uid="{D9102D15-FF01-1040-86BC-7CD746DF5EA2}"/>
+    <workbookView xWindow="300" yWindow="500" windowWidth="26700" windowHeight="16280" xr2:uid="{D9102D15-FF01-1040-86BC-7CD746DF5EA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$J$6</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -53,12 +56,6 @@
     <t>Treatment</t>
   </si>
   <si>
-    <t>Ambient</t>
-  </si>
-  <si>
-    <t>Hot</t>
-  </si>
-  <si>
     <t>Percent Healed</t>
   </si>
   <si>
@@ -71,20 +68,42 @@
     <t xml:space="preserve"> Ferets Diameter</t>
   </si>
   <si>
-    <t xml:space="preserve">n </t>
+    <t>Ambient (n= 6)</t>
+  </si>
+  <si>
+    <t>± Percent Healed SD</t>
+  </si>
+  <si>
+    <t>Hot  (n=5)</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Table 1.  </t>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Table 3.</t>
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <b/>
+        <sz val="11"/>
         <color theme="1"/>
         <rFont val="Aptos Narrow"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Mean fragment wound area (mm2), mean perimeter (mm), and mean ferets diameter (mm) with standard deviations at day 0, 1, 10, and 19.  Sample size (n) decreases by day 19 as fully healed corals were removed from analysis. </t>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mean fragment wound area (mm2),  perimeter (mm), and  ferets diameter (mm) with standard deviations at day 0, 1, 10, and 19.  Mean percent healed is calculated by taking the difference in  area from  initial area and dividing by initial area  for each timepoint.  Sample size is 6 and 5 for ambient and hot treatments, respectively. </t>
     </r>
   </si>
 </sst>
@@ -95,19 +114,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -123,11 +135,28 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -139,7 +168,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -167,11 +196,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -180,42 +218,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -224,38 +279,168 @@
   </cellStyles>
   <dxfs count="14">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -267,18 +452,6 @@
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -299,7 +472,7 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>615950</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="65" cy="172227"/>
@@ -354,8 +527,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E393AD3F-75F8-7B4D-9999-0617A1BAABA9}" name="Table3" displayName="Table3" ref="B3:J11" headerRowDxfId="13" dataDxfId="12" totalsRowDxfId="11" headerRowBorderDxfId="10">
-  <autoFilter ref="B3:J11" xr:uid="{E393AD3F-75F8-7B4D-9999-0617A1BAABA9}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E393AD3F-75F8-7B4D-9999-0617A1BAABA9}" name="Table3" displayName="Table3" ref="B4:J12" headerRowDxfId="2" dataDxfId="0" totalsRowDxfId="1" headerRowBorderDxfId="13">
+  <autoFilter ref="B4:J12" xr:uid="{E393AD3F-75F8-7B4D-9999-0617A1BAABA9}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -367,15 +540,15 @@
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{42F7ADB4-3B52-E443-933F-D0416CD21B88}" name="Day" totalsRowLabel="Total" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{FF937BBA-A3A1-A447-92E0-9F99FF215B42}" name=" Area" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{AC8680A9-B511-6247-9835-530FBD9482EC}" name="± Area SD" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{54AE447D-2035-014F-9BA2-424CDDFFD71C}" name=" Perimeter" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{6D47506F-BC59-614E-A99B-7C1DA516AFCA}" name="± Perimeter SD" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{F65D9021-4A7F-6645-B9C2-1B1EBFB0B1E1}" name=" Ferets Diameter" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{C45B19B1-2C21-814A-BDD9-E9BC4D597A64}" name="± Ferets Diameter SD" totalsRowFunction="sum" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{A479872A-4329-094A-A337-03085FAB73FD}" name="Percent Healed" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{FCDC031F-7942-F84F-A708-9650CCE75B63}" name="n " dataDxfId="0" totalsRowDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{42F7ADB4-3B52-E443-933F-D0416CD21B88}" name="Day" totalsRowLabel="Total" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{FF937BBA-A3A1-A447-92E0-9F99FF215B42}" name=" Area" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{AC8680A9-B511-6247-9835-530FBD9482EC}" name="± Area SD" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{54AE447D-2035-014F-9BA2-424CDDFFD71C}" name=" Perimeter" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{6D47506F-BC59-614E-A99B-7C1DA516AFCA}" name="± Perimeter SD" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{F65D9021-4A7F-6645-B9C2-1B1EBFB0B1E1}" name=" Ferets Diameter" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{C45B19B1-2C21-814A-BDD9-E9BC4D597A64}" name="± Ferets Diameter SD" totalsRowFunction="sum" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{A479872A-4329-094A-A337-03085FAB73FD}" name="Percent Healed" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{FCDC031F-7942-F84F-A708-9650CCE75B63}" name="± Percent Healed SD" dataDxfId="3" totalsRowDxfId="12"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -698,37 +871,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8788338E-1A10-B343-80A5-9E547DD0CE78}">
-  <dimension ref="A1:T22"/>
+  <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection sqref="A1:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" customWidth="1"/>
-    <col min="7" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="10" t="s">
+      <c r="A1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
@@ -739,84 +915,59 @@
       <c r="T1" s="3"/>
     </row>
     <row r="2" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
+    <row r="3" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5">
-        <v>20.495333333333299</v>
-      </c>
-      <c r="D4" s="5">
-        <v>6.4743024540614904</v>
-      </c>
-      <c r="E4" s="5">
-        <v>22.989333333333299</v>
-      </c>
-      <c r="F4" s="5">
-        <v>4.0001640799680498</v>
-      </c>
-      <c r="G4" s="5">
-        <v>7.0298333333333298</v>
-      </c>
-      <c r="H4" s="5">
-        <v>1.21143739692428</v>
-      </c>
-      <c r="I4" s="5">
-        <v>0</v>
-      </c>
-      <c r="J4" s="16">
-        <v>6</v>
+      <c r="J4" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -826,33 +977,35 @@
       <c r="S4" s="2"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
+      <c r="A5" s="11" t="s">
+        <v>9</v>
+      </c>
       <c r="B5" s="4">
-        <v>1</v>
-      </c>
-      <c r="C5" s="5">
-        <v>19.018000000000001</v>
-      </c>
-      <c r="D5" s="5">
-        <v>5.8696917806644704</v>
-      </c>
-      <c r="E5" s="5">
-        <v>21.4226666666667</v>
-      </c>
-      <c r="F5" s="5">
-        <v>4.6477378009808898</v>
-      </c>
-      <c r="G5" s="5">
-        <v>6.5158333333333296</v>
-      </c>
-      <c r="H5" s="5">
-        <v>1.7253499838197099</v>
-      </c>
-      <c r="I5" s="5">
-        <v>7.2081449435642302</v>
-      </c>
-      <c r="J5" s="16">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="C5" s="12">
+        <v>20.495333333333299</v>
+      </c>
+      <c r="D5" s="12">
+        <v>6.4743024540614904</v>
+      </c>
+      <c r="E5" s="12">
+        <v>22.989333333333299</v>
+      </c>
+      <c r="F5" s="12">
+        <v>4.0001640799680498</v>
+      </c>
+      <c r="G5" s="12">
+        <v>7.0298333333333298</v>
+      </c>
+      <c r="H5" s="12">
+        <v>1.21143739692428</v>
+      </c>
+      <c r="I5" s="12">
+        <v>0</v>
+      </c>
+      <c r="J5" s="12">
+        <v>0</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -864,31 +1017,31 @@
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="11"/>
       <c r="B6" s="4">
-        <v>10</v>
-      </c>
-      <c r="C6" s="5">
-        <v>15.096</v>
-      </c>
-      <c r="D6" s="5">
-        <v>8.5084957072328606</v>
-      </c>
-      <c r="E6" s="5">
-        <v>16.116333333333301</v>
-      </c>
-      <c r="F6" s="5">
-        <v>5.6545191720133596</v>
-      </c>
-      <c r="G6" s="5">
-        <v>5.4438333333333304</v>
-      </c>
-      <c r="H6" s="5">
-        <v>2.0960917362240301</v>
-      </c>
-      <c r="I6" s="5">
-        <v>26.344208437693013</v>
-      </c>
-      <c r="J6" s="16">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="C6" s="12">
+        <v>19.018000000000001</v>
+      </c>
+      <c r="D6" s="12">
+        <v>5.8696917806644704</v>
+      </c>
+      <c r="E6" s="12">
+        <v>21.4226666666667</v>
+      </c>
+      <c r="F6" s="12">
+        <v>4.6477378009808898</v>
+      </c>
+      <c r="G6" s="12">
+        <v>6.5158333333333296</v>
+      </c>
+      <c r="H6" s="12">
+        <v>1.7253499838197099</v>
+      </c>
+      <c r="I6" s="6">
+        <v>5.52816025649736</v>
+      </c>
+      <c r="J6" s="18">
+        <v>15.090301563587101</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -900,31 +1053,31 @@
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="11"/>
       <c r="B7" s="4">
-        <v>19</v>
-      </c>
-      <c r="C7" s="5">
-        <v>2.9076666666666702</v>
-      </c>
-      <c r="D7" s="5">
-        <v>4.5198626822799204</v>
-      </c>
-      <c r="E7" s="5">
-        <v>3.74833333333333</v>
-      </c>
-      <c r="F7" s="5">
-        <v>5.80982893609327</v>
-      </c>
-      <c r="G7" s="5">
-        <v>1.2515000000000001</v>
-      </c>
-      <c r="H7" s="5">
-        <v>1.9398160479798101</v>
-      </c>
-      <c r="I7" s="5">
-        <v>85.813030608593778</v>
-      </c>
-      <c r="J7" s="16">
-        <v>2</v>
+        <v>10</v>
+      </c>
+      <c r="C7" s="12">
+        <v>15.096</v>
+      </c>
+      <c r="D7" s="12">
+        <v>8.5084957072328606</v>
+      </c>
+      <c r="E7" s="12">
+        <v>16.116333333333301</v>
+      </c>
+      <c r="F7" s="12">
+        <v>5.6545191720133596</v>
+      </c>
+      <c r="G7" s="12">
+        <v>5.4438333333333304</v>
+      </c>
+      <c r="H7" s="12">
+        <v>2.0960917362240301</v>
+      </c>
+      <c r="I7" s="6">
+        <v>25.6310153105781</v>
+      </c>
+      <c r="J7" s="13">
+        <v>31.812760463564299</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -934,35 +1087,33 @@
       <c r="S7" s="2"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
-        <v>6</v>
-      </c>
+      <c r="A8" s="11"/>
       <c r="B8" s="4">
-        <v>0</v>
-      </c>
-      <c r="C8" s="5">
-        <v>23.9742</v>
-      </c>
-      <c r="D8" s="5">
-        <v>10.8535630416928</v>
-      </c>
-      <c r="E8" s="5">
-        <v>22.960999999999999</v>
-      </c>
-      <c r="F8" s="5">
-        <v>7.2544776517679104</v>
-      </c>
-      <c r="G8" s="5">
-        <v>7.0175999999999998</v>
-      </c>
-      <c r="H8" s="5">
-        <v>1.77008002643948</v>
-      </c>
-      <c r="I8" s="5">
-        <v>0</v>
-      </c>
-      <c r="J8" s="16">
-        <v>5</v>
+        <v>19</v>
+      </c>
+      <c r="C8" s="12">
+        <v>2.9076666666666702</v>
+      </c>
+      <c r="D8" s="12">
+        <v>4.5198626822799204</v>
+      </c>
+      <c r="E8" s="12">
+        <v>3.74833333333333</v>
+      </c>
+      <c r="F8" s="12">
+        <v>5.80982893609327</v>
+      </c>
+      <c r="G8" s="12">
+        <v>1.2515000000000001</v>
+      </c>
+      <c r="H8" s="12">
+        <v>1.9398160479798101</v>
+      </c>
+      <c r="I8" s="6">
+        <v>86.247196064770904</v>
+      </c>
+      <c r="J8" s="13">
+        <v>21.819120869759399</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -972,33 +1123,35 @@
       <c r="S8" s="2"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A9" s="12"/>
-      <c r="B9" s="4">
-        <v>1</v>
-      </c>
-      <c r="C9" s="5">
-        <v>24.5396</v>
-      </c>
-      <c r="D9" s="5">
-        <v>9.5742915821485202</v>
-      </c>
-      <c r="E9" s="5">
-        <v>21.980799999999999</v>
-      </c>
-      <c r="F9" s="5">
-        <v>5.7104530643373597</v>
-      </c>
-      <c r="G9" s="5">
-        <v>6.7186000000000003</v>
-      </c>
-      <c r="H9" s="5">
-        <v>1.4394920284600401</v>
-      </c>
-      <c r="I9" s="5">
-        <v>-2.358368579556358</v>
-      </c>
-      <c r="J9" s="16">
-        <v>5</v>
+      <c r="A9" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="19">
+        <v>0</v>
+      </c>
+      <c r="C9" s="20">
+        <v>23.9742</v>
+      </c>
+      <c r="D9" s="20">
+        <v>10.8535630416928</v>
+      </c>
+      <c r="E9" s="20">
+        <v>22.960999999999999</v>
+      </c>
+      <c r="F9" s="20">
+        <v>7.2544776517679104</v>
+      </c>
+      <c r="G9" s="20">
+        <v>7.0175999999999998</v>
+      </c>
+      <c r="H9" s="20">
+        <v>1.77008002643948</v>
+      </c>
+      <c r="I9" s="20">
+        <v>0</v>
+      </c>
+      <c r="J9" s="20">
+        <v>0</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -1008,33 +1161,33 @@
       <c r="S9" s="2"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A10" s="12"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="4">
-        <v>10</v>
-      </c>
-      <c r="C10" s="5">
-        <v>20.2332</v>
-      </c>
-      <c r="D10" s="5">
-        <v>11.1217104215134</v>
-      </c>
-      <c r="E10" s="5">
-        <v>19.075399999999998</v>
-      </c>
-      <c r="F10" s="5">
-        <v>5.3057389023584598</v>
-      </c>
-      <c r="G10" s="5">
-        <v>6.2122000000000002</v>
-      </c>
-      <c r="H10" s="5">
-        <v>1.3113247881436501</v>
-      </c>
-      <c r="I10" s="5">
-        <v>15.604274595189827</v>
-      </c>
-      <c r="J10" s="16">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="C10" s="12">
+        <v>24.5396</v>
+      </c>
+      <c r="D10" s="12">
+        <v>9.5742915821485202</v>
+      </c>
+      <c r="E10" s="12">
+        <v>21.980799999999999</v>
+      </c>
+      <c r="F10" s="12">
+        <v>5.7104530643373597</v>
+      </c>
+      <c r="G10" s="12">
+        <v>6.7186000000000003</v>
+      </c>
+      <c r="H10" s="12">
+        <v>1.4394920284600401</v>
+      </c>
+      <c r="I10" s="13">
+        <v>-7.1609759706650999</v>
+      </c>
+      <c r="J10" s="13">
+        <v>20.9276548500718</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -1044,52 +1197,83 @@
       <c r="S10" s="2"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
-      <c r="B11" s="8">
+      <c r="A11" s="22"/>
+      <c r="B11" s="4">
+        <v>10</v>
+      </c>
+      <c r="C11" s="12">
+        <v>20.2332</v>
+      </c>
+      <c r="D11" s="12">
+        <v>11.1217104215134</v>
+      </c>
+      <c r="E11" s="12">
+        <v>19.075399999999998</v>
+      </c>
+      <c r="F11" s="12">
+        <v>5.3057389023584598</v>
+      </c>
+      <c r="G11" s="12">
+        <v>6.2122000000000002</v>
+      </c>
+      <c r="H11" s="12">
+        <v>1.3113247881436501</v>
+      </c>
+      <c r="I11" s="13">
+        <v>11.4095913858073</v>
+      </c>
+      <c r="J11" s="13">
+        <v>31.559298327212499</v>
+      </c>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A12" s="14"/>
+      <c r="B12" s="15">
         <v>19</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C12" s="16">
         <v>8.0144000000000002</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D12" s="16">
         <v>13.4274372387288</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E12" s="16">
         <v>6.8231999999999999</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F12" s="16">
         <v>9.9234232853385809</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G12" s="16">
         <v>2.2376</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H12" s="16">
         <v>3.2011265673197</v>
       </c>
-      <c r="I11" s="9">
-        <v>66.570730201633424</v>
-      </c>
-      <c r="J11" s="17">
-        <v>2</v>
+      <c r="I12" s="17">
+        <v>73.547028485494593</v>
+      </c>
+      <c r="J12" s="17">
+        <v>37.443993001096402</v>
       </c>
     </row>
-    <row r="20" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L20" s="6"/>
-    </row>
-    <row r="21" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L21" s="6"/>
-    </row>
-    <row r="22" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L22" s="6"/>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A12"/>
     <mergeCell ref="M1:T1"/>
-    <mergeCell ref="B1:J2"/>
+    <mergeCell ref="A1:J3"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
reanalyzing regen data, results: figures and tables
</commit_message>
<xml_diff>
--- a/Wound_Closure/Output/summary.table.combined.xlsx
+++ b/Wound_Closure/Output/summary.table.combined.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninahmunk/Desktop/Projects/Acropora_Regeneration-main/Wound_Closure/Output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5BFEC20-958F-3A49-85EE-529919CACE6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F15E57-268A-3F42-A036-7C04FA02ABE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="500" windowWidth="26700" windowHeight="16280" xr2:uid="{D9102D15-FF01-1040-86BC-7CD746DF5EA2}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$J$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -209,15 +210,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -226,58 +224,58 @@
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -289,6 +287,7 @@
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -302,7 +301,138 @@
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -317,141 +447,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -527,7 +522,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E393AD3F-75F8-7B4D-9999-0617A1BAABA9}" name="Table3" displayName="Table3" ref="B4:J12" headerRowDxfId="2" dataDxfId="0" totalsRowDxfId="1" headerRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E393AD3F-75F8-7B4D-9999-0617A1BAABA9}" name="Table3" displayName="Table3" ref="B4:J12" headerRowDxfId="13" dataDxfId="11" totalsRowDxfId="10" headerRowBorderDxfId="12">
   <autoFilter ref="B4:J12" xr:uid="{E393AD3F-75F8-7B4D-9999-0617A1BAABA9}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -540,15 +535,15 @@
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{42F7ADB4-3B52-E443-933F-D0416CD21B88}" name="Day" totalsRowLabel="Total" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{FF937BBA-A3A1-A447-92E0-9F99FF215B42}" name=" Area" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{AC8680A9-B511-6247-9835-530FBD9482EC}" name="± Area SD" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{54AE447D-2035-014F-9BA2-424CDDFFD71C}" name=" Perimeter" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{6D47506F-BC59-614E-A99B-7C1DA516AFCA}" name="± Perimeter SD" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{F65D9021-4A7F-6645-B9C2-1B1EBFB0B1E1}" name=" Ferets Diameter" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{C45B19B1-2C21-814A-BDD9-E9BC4D597A64}" name="± Ferets Diameter SD" totalsRowFunction="sum" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{A479872A-4329-094A-A337-03085FAB73FD}" name="Percent Healed" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{FCDC031F-7942-F84F-A708-9650CCE75B63}" name="± Percent Healed SD" dataDxfId="3" totalsRowDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{42F7ADB4-3B52-E443-933F-D0416CD21B88}" name="Day" totalsRowLabel="Total" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{FF937BBA-A3A1-A447-92E0-9F99FF215B42}" name=" Area" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{AC8680A9-B511-6247-9835-530FBD9482EC}" name="± Area SD" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{54AE447D-2035-014F-9BA2-424CDDFFD71C}" name=" Perimeter" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{6D47506F-BC59-614E-A99B-7C1DA516AFCA}" name="± Perimeter SD" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{F65D9021-4A7F-6645-B9C2-1B1EBFB0B1E1}" name=" Ferets Diameter" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{C45B19B1-2C21-814A-BDD9-E9BC4D597A64}" name="± Ferets Diameter SD" totalsRowFunction="sum" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{A479872A-4329-094A-A337-03085FAB73FD}" name="Percent Healed" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{FCDC031F-7942-F84F-A708-9650CCE75B63}" name="± Percent Healed SD" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -874,7 +869,7 @@
   <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J12"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -893,80 +888,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
     </row>
     <row r="2" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="N4" s="2"/>
@@ -977,34 +972,34 @@
       <c r="S4" s="2"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>0</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="8">
         <v>20.495333333333299</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="8">
         <v>6.4743024540614904</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="8">
         <v>22.989333333333299</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="8">
         <v>4.0001640799680498</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="8">
         <v>7.0298333333333298</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="8">
         <v>1.21143739692428</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="8">
         <v>0</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="8">
         <v>0</v>
       </c>
       <c r="N5" s="2"/>
@@ -1015,32 +1010,32 @@
       <c r="S5" s="2"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
-      <c r="B6" s="4">
+      <c r="A6" s="15"/>
+      <c r="B6" s="3">
         <v>1</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="8">
         <v>19.018000000000001</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="8">
         <v>5.8696917806644704</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="8">
         <v>21.4226666666667</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="8">
         <v>4.6477378009808898</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="8">
         <v>6.5158333333333296</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="8">
         <v>1.7253499838197099</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="5">
         <v>5.52816025649736</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="9">
         <v>15.090301563587101</v>
       </c>
       <c r="N6" s="2"/>
@@ -1051,32 +1046,32 @@
       <c r="S6" s="2"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
-      <c r="B7" s="4">
+      <c r="A7" s="15"/>
+      <c r="B7" s="3">
         <v>10</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="8">
         <v>15.096</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="8">
         <v>8.5084957072328606</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="8">
         <v>16.116333333333301</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="8">
         <v>5.6545191720133596</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="8">
         <v>5.4438333333333304</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="8">
         <v>2.0960917362240301</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="5">
         <v>25.6310153105781</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="9">
         <v>31.812760463564299</v>
       </c>
       <c r="N7" s="2"/>
@@ -1087,32 +1082,32 @@
       <c r="S7" s="2"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
-      <c r="B8" s="4">
+      <c r="A8" s="15"/>
+      <c r="B8" s="3">
         <v>19</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="8">
         <v>2.9076666666666702</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="8">
         <v>4.5198626822799204</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="8">
         <v>3.74833333333333</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="8">
         <v>5.80982893609327</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="8">
         <v>1.2515000000000001</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="8">
         <v>1.9398160479798101</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="5">
         <v>86.247196064770904</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="9">
         <v>21.819120869759399</v>
       </c>
       <c r="N8" s="2"/>
@@ -1123,34 +1118,34 @@
       <c r="S8" s="2"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="13">
         <v>0</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="14">
         <v>23.9742</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="14">
         <v>10.8535630416928</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="14">
         <v>22.960999999999999</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="14">
         <v>7.2544776517679104</v>
       </c>
-      <c r="G9" s="20">
+      <c r="G9" s="14">
         <v>7.0175999999999998</v>
       </c>
-      <c r="H9" s="20">
+      <c r="H9" s="14">
         <v>1.77008002643948</v>
       </c>
-      <c r="I9" s="20">
+      <c r="I9" s="14">
         <v>0</v>
       </c>
-      <c r="J9" s="20">
+      <c r="J9" s="14">
         <v>0</v>
       </c>
       <c r="N9" s="2"/>
@@ -1161,32 +1156,32 @@
       <c r="S9" s="2"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A10" s="22"/>
-      <c r="B10" s="4">
+      <c r="A10" s="15"/>
+      <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="8">
         <v>24.5396</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="8">
         <v>9.5742915821485202</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="8">
         <v>21.980799999999999</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="8">
         <v>5.7104530643373597</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="8">
         <v>6.7186000000000003</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="8">
         <v>1.4394920284600401</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="9">
         <v>-7.1609759706650999</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="9">
         <v>20.9276548500718</v>
       </c>
       <c r="N10" s="2"/>
@@ -1197,32 +1192,32 @@
       <c r="S10" s="2"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A11" s="22"/>
-      <c r="B11" s="4">
+      <c r="A11" s="15"/>
+      <c r="B11" s="3">
         <v>10</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="8">
         <v>20.2332</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="8">
         <v>11.1217104215134</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="8">
         <v>19.075399999999998</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="8">
         <v>5.3057389023584598</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="8">
         <v>6.2122000000000002</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="8">
         <v>1.3113247881436501</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="9">
         <v>11.4095913858073</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="9">
         <v>31.559298327212499</v>
       </c>
       <c r="N11" s="2"/>
@@ -1233,38 +1228,38 @@
       <c r="S11" s="2"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15">
+      <c r="A12" s="17"/>
+      <c r="B12" s="10">
         <v>19</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="11">
         <v>8.0144000000000002</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="11">
         <v>13.4274372387288</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="11">
         <v>6.8231999999999999</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="11">
         <v>9.9234232853385809</v>
       </c>
-      <c r="G12" s="16">
+      <c r="G12" s="11">
         <v>2.2376</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12" s="11">
         <v>3.2011265673197</v>
       </c>
-      <c r="I12" s="17">
+      <c r="I12" s="12">
         <v>73.547028485494593</v>
       </c>
-      <c r="J12" s="17">
+      <c r="J12" s="12">
         <v>37.443993001096402</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>